<commit_message>
Fixed a link or two in the parts list.
</commit_message>
<xml_diff>
--- a/parts.xlsx
+++ b/parts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github_projects\twitchy_cat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBA123C3-2B06-4DD3-B74F-39B8CE4CC6B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEFC13F8-6225-4633-969C-39B4FBBB042B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2563" yWindow="926" windowWidth="19680" windowHeight="15068" xr2:uid="{F21D823E-D158-4F0D-A6E0-D13332463531}"/>
+    <workbookView xWindow="7474" yWindow="1234" windowWidth="19680" windowHeight="15069" xr2:uid="{F21D823E-D158-4F0D-A6E0-D13332463531}"/>
   </bookViews>
   <sheets>
     <sheet name="Twitchy Cat" sheetId="1" r:id="rId1"/>
@@ -577,7 +577,7 @@
   <dimension ref="A1:R28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -585,6 +585,7 @@
     <col min="1" max="1" width="14.765625" customWidth="1"/>
     <col min="2" max="2" width="4" customWidth="1"/>
     <col min="3" max="3" width="15.69140625" customWidth="1"/>
+    <col min="4" max="4" width="18.3046875" customWidth="1"/>
     <col min="5" max="5" width="10.61328125" customWidth="1"/>
     <col min="7" max="7" width="8.07421875" customWidth="1"/>
     <col min="9" max="10" width="10.3046875" customWidth="1"/>
@@ -604,7 +605,7 @@
         <v>17</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.4">
@@ -666,55 +667,55 @@
       <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5" s="1">
-        <v>17.989999999999998</v>
+        <v>17.670000000000002</v>
       </c>
       <c r="G5" s="1">
         <v>0</v>
       </c>
       <c r="H5" s="1">
         <f>10.75% * (F5 + G5)</f>
-        <v>1.9339249999999999</v>
+        <v>1.8995250000000001</v>
       </c>
       <c r="I5" s="2">
         <f>SUM(F5:H5)</f>
-        <v>19.923924999999997</v>
+        <v>19.569525000000002</v>
       </c>
       <c r="J5" s="2">
         <f>I5/E5</f>
-        <v>19.923924999999997</v>
+        <v>19.569525000000002</v>
       </c>
       <c r="K5">
         <v>1</v>
       </c>
       <c r="L5" s="2">
         <f>J5*K5</f>
-        <v>19.923924999999997</v>
+        <v>19.569525000000002</v>
       </c>
       <c r="M5">
         <f>$B$2*K5</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="N5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O5">
         <f>MAX(M5 - N5, 0)</f>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="P5">
         <f>CEILING(O5/E5, 1)</f>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="Q5" s="2">
         <f>I5*P5</f>
-        <v>159.39139999999998</v>
+        <v>215.26477500000001</v>
       </c>
       <c r="R5">
         <f>E5*P5 +N5 - M5</f>
@@ -725,47 +726,47 @@
       <c r="C6" t="s">
         <v>46</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="5" t="s">
         <v>19</v>
       </c>
       <c r="E6">
         <v>4</v>
       </c>
       <c r="F6" s="1">
-        <v>19.989999999999998</v>
+        <v>16.989999999999998</v>
       </c>
       <c r="G6" s="1">
         <v>0</v>
       </c>
       <c r="H6" s="1">
         <f>10.75% * (F6 + G6)</f>
-        <v>2.1489249999999998</v>
+        <v>1.8264249999999997</v>
       </c>
       <c r="I6" s="2">
         <f>SUM(F6:H6)</f>
-        <v>22.138924999999997</v>
+        <v>18.816424999999999</v>
       </c>
       <c r="J6" s="2">
         <f>I6/E6</f>
-        <v>5.5347312499999992</v>
+        <v>4.7041062499999997</v>
       </c>
       <c r="K6">
         <v>1</v>
       </c>
       <c r="L6" s="2">
         <f>J6*K6</f>
-        <v>5.5347312499999992</v>
+        <v>4.7041062499999997</v>
       </c>
       <c r="M6">
         <f>$B$2*K6</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="N6">
         <v>4</v>
       </c>
       <c r="O6">
         <f>MAX(M6 - N6, 0)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="P6">
         <f>CEILING(O6/E6, 1)</f>
@@ -773,18 +774,18 @@
       </c>
       <c r="Q6" s="2">
         <f>I6*P6</f>
-        <v>44.277849999999994</v>
+        <v>37.632849999999998</v>
       </c>
       <c r="R6">
         <f>E6*P6 +N6 - M6</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.4">
       <c r="C7" t="s">
         <v>21</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="5" t="s">
         <v>20</v>
       </c>
       <c r="E7">
@@ -817,22 +818,22 @@
       </c>
       <c r="M7">
         <f>$B$2*K7</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="N7">
         <v>6</v>
       </c>
       <c r="O7">
         <f>MAX(M7 - N7, 0)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P7">
         <f>CEILING(O7/E7, 1)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q7" s="2">
         <f>I7*P7</f>
-        <v>6.0248000000000008</v>
+        <v>9.0372000000000021</v>
       </c>
       <c r="R7">
         <f>E7*P7 +N7 - M7</f>
@@ -876,14 +877,14 @@
       </c>
       <c r="M8">
         <f>$B$2*K8</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="N8">
         <v>3</v>
       </c>
       <c r="O8">
         <f>MAX(M8 - N8, 0)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="P8">
         <f>CEILING(O8/E8, 1)</f>
@@ -895,7 +896,7 @@
       </c>
       <c r="R8">
         <f>E8*P8 +N8 - M8</f>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.4">
@@ -927,34 +928,34 @@
         <v>5.5264250000000008E-2</v>
       </c>
       <c r="K9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L9" s="2">
         <f>J9*K9</f>
-        <v>0.11052850000000002</v>
+        <v>0.22105700000000003</v>
       </c>
       <c r="M9">
         <f>$B$2*K9</f>
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="N9">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="O9">
         <f>MAX(M9 - N9, 0)</f>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="P9">
         <f>CEILING(O9/E9, 1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q9" s="2">
         <f>I9*P9</f>
-        <v>5.5264250000000006</v>
+        <v>0</v>
       </c>
       <c r="R9">
         <f>E9*P9 +N9 - M9</f>
-        <v>80</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.4">
@@ -991,51 +992,51 @@
         <v>1</v>
       </c>
       <c r="F12" s="1">
-        <v>14.98</v>
+        <v>15.99</v>
       </c>
       <c r="G12" s="1">
         <v>0</v>
       </c>
       <c r="H12" s="1">
-        <f>10.75% * (F12 + G12)</f>
-        <v>1.6103499999999999</v>
+        <f t="shared" ref="H12:H18" si="0">10.75% * (F12 + G12)</f>
+        <v>1.718925</v>
       </c>
       <c r="I12" s="2">
-        <f>SUM(F12:H12)</f>
-        <v>16.590350000000001</v>
+        <f t="shared" ref="I12:I18" si="1">SUM(F12:H12)</f>
+        <v>17.708925000000001</v>
       </c>
       <c r="J12" s="2">
-        <f>IF(E12&gt;0, I12/E12, 0)</f>
-        <v>16.590350000000001</v>
+        <f t="shared" ref="J12:J18" si="2">IF(E12&gt;0, I12/E12, 0)</f>
+        <v>17.708925000000001</v>
       </c>
       <c r="K12">
         <v>1</v>
       </c>
       <c r="L12" s="2">
-        <f>J12*K12</f>
-        <v>16.590350000000001</v>
+        <f t="shared" ref="L12:L18" si="3">J12*K12</f>
+        <v>17.708925000000001</v>
       </c>
       <c r="M12">
-        <f>$B$2*K12</f>
-        <v>10</v>
+        <f t="shared" ref="M12:M18" si="4">$B$2*K12</f>
+        <v>12</v>
       </c>
       <c r="N12">
         <v>0</v>
       </c>
       <c r="O12">
-        <f>MAX(M12 - N12, 0)</f>
-        <v>10</v>
+        <f t="shared" ref="O12:O18" si="5">MAX(M12 - N12, 0)</f>
+        <v>12</v>
       </c>
       <c r="P12">
-        <f>CEILING(O12/E12, 1)</f>
-        <v>10</v>
+        <f t="shared" ref="P12:P18" si="6">CEILING(O12/E12, 1)</f>
+        <v>12</v>
       </c>
       <c r="Q12" s="2">
-        <f>I12*P12</f>
-        <v>165.90350000000001</v>
+        <f t="shared" ref="Q12:Q18" si="7">I12*P12</f>
+        <v>212.50710000000001</v>
       </c>
       <c r="R12">
-        <f>E12*P12 +N12 - M12</f>
+        <f t="shared" ref="R12:R18" si="8">E12*P12 +N12 - M12</f>
         <v>0</v>
       </c>
     </row>
@@ -1056,45 +1057,45 @@
         <v>0</v>
       </c>
       <c r="H13" s="1">
-        <f>10.75% * (F13 + G13)</f>
+        <f t="shared" si="0"/>
         <v>0.96642499999999998</v>
       </c>
       <c r="I13" s="2">
-        <f>SUM(F13:H13)</f>
+        <f t="shared" si="1"/>
         <v>9.9564249999999994</v>
       </c>
       <c r="J13" s="2">
-        <f>IF(E13&gt;0, I13/E13, 0)</f>
+        <f t="shared" si="2"/>
         <v>4.9782124999999997</v>
       </c>
       <c r="K13">
         <v>1</v>
       </c>
       <c r="L13" s="2">
-        <f>J13*K13</f>
+        <f t="shared" si="3"/>
         <v>4.9782124999999997</v>
       </c>
       <c r="M13">
-        <f>$B$2*K13</f>
-        <v>10</v>
+        <f t="shared" si="4"/>
+        <v>12</v>
       </c>
       <c r="N13">
         <v>0</v>
       </c>
       <c r="O13">
-        <f>MAX(M13 - N13, 0)</f>
-        <v>10</v>
+        <f t="shared" si="5"/>
+        <v>12</v>
       </c>
       <c r="P13">
-        <f>CEILING(O13/E13, 1)</f>
-        <v>5</v>
+        <f t="shared" si="6"/>
+        <v>6</v>
       </c>
       <c r="Q13" s="2">
-        <f>I13*P13</f>
-        <v>49.782124999999994</v>
+        <f t="shared" si="7"/>
+        <v>59.738549999999996</v>
       </c>
       <c r="R13">
-        <f>E13*P13 +N13 - M13</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -1102,7 +1103,7 @@
       <c r="C14" t="s">
         <v>27</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="5" t="s">
         <v>28</v>
       </c>
       <c r="E14">
@@ -1115,112 +1116,112 @@
         <v>0</v>
       </c>
       <c r="H14" s="1">
-        <f>10.75% * (F14 + G14)</f>
+        <f t="shared" si="0"/>
         <v>1.0535000000000001</v>
       </c>
       <c r="I14" s="2">
-        <f>SUM(F14:H14)</f>
+        <f t="shared" si="1"/>
         <v>10.8535</v>
       </c>
       <c r="J14" s="2">
-        <f>IF(E14&gt;0, I14/E14, 0)</f>
+        <f t="shared" si="2"/>
         <v>1.08535</v>
       </c>
       <c r="K14">
         <v>2</v>
       </c>
       <c r="L14" s="2">
-        <f>J14*K14</f>
+        <f t="shared" si="3"/>
         <v>2.1707000000000001</v>
       </c>
       <c r="M14">
-        <f>$B$2*K14</f>
-        <v>20</v>
+        <f t="shared" si="4"/>
+        <v>24</v>
       </c>
       <c r="N14">
         <v>10</v>
       </c>
       <c r="O14">
-        <f>MAX(M14 - N14, 0)</f>
-        <v>10</v>
+        <f t="shared" si="5"/>
+        <v>14</v>
       </c>
       <c r="P14">
-        <f>CEILING(O14/E14, 1)</f>
-        <v>1</v>
+        <f t="shared" si="6"/>
+        <v>2</v>
       </c>
       <c r="Q14" s="2">
-        <f>I14*P14</f>
-        <v>10.8535</v>
+        <f t="shared" si="7"/>
+        <v>21.707000000000001</v>
       </c>
       <c r="R14">
-        <f>E14*P14 +N14 - M14</f>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.4">
       <c r="C15" t="s">
         <v>33</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="5" t="s">
         <v>34</v>
       </c>
       <c r="E15">
         <v>10</v>
       </c>
       <c r="F15" s="1">
-        <v>9.39</v>
+        <v>10.09</v>
       </c>
       <c r="G15" s="1">
         <v>0</v>
       </c>
       <c r="H15" s="1">
-        <f>10.75% * (F15 + G15)</f>
-        <v>1.009425</v>
+        <f t="shared" si="0"/>
+        <v>1.0846750000000001</v>
       </c>
       <c r="I15" s="2">
-        <f>SUM(F15:H15)</f>
-        <v>10.399425000000001</v>
+        <f t="shared" si="1"/>
+        <v>11.174675000000001</v>
       </c>
       <c r="J15" s="2">
-        <f>IF(E15&gt;0, I15/E15, 0)</f>
-        <v>1.0399425</v>
+        <f t="shared" si="2"/>
+        <v>1.1174675000000001</v>
       </c>
       <c r="K15">
         <v>1</v>
       </c>
       <c r="L15" s="2">
-        <f>J15*K15</f>
-        <v>1.0399425</v>
+        <f t="shared" si="3"/>
+        <v>1.1174675000000001</v>
       </c>
       <c r="M15">
-        <f>$B$2*K15</f>
-        <v>10</v>
+        <f t="shared" si="4"/>
+        <v>12</v>
       </c>
       <c r="N15">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="O15">
-        <f>MAX(M15 - N15, 0)</f>
-        <v>2</v>
+        <f t="shared" si="5"/>
+        <v>5</v>
       </c>
       <c r="P15">
-        <f>CEILING(O15/E15, 1)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="Q15" s="2">
-        <f>I15*P15</f>
-        <v>10.399425000000001</v>
+        <f t="shared" si="7"/>
+        <v>11.174675000000001</v>
       </c>
       <c r="R15">
-        <f>E15*P15 +N15 - M15</f>
-        <v>8</v>
+        <f t="shared" si="8"/>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.4">
       <c r="C16" t="s">
         <v>35</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="5" t="s">
         <v>36</v>
       </c>
       <c r="E16">
@@ -1233,46 +1234,46 @@
         <v>0</v>
       </c>
       <c r="H16" s="1">
-        <f>10.75% * (F16 + G16)</f>
+        <f t="shared" si="0"/>
         <v>0.53642500000000004</v>
       </c>
       <c r="I16" s="2">
-        <f>SUM(F16:H16)</f>
+        <f t="shared" si="1"/>
         <v>5.5264250000000006</v>
       </c>
       <c r="J16" s="2">
-        <f>IF(E16&gt;0, I16/E16, 0)</f>
+        <f t="shared" si="2"/>
         <v>0.55264250000000004</v>
       </c>
       <c r="K16">
         <v>1</v>
       </c>
       <c r="L16" s="2">
-        <f>J16*K16</f>
+        <f t="shared" si="3"/>
         <v>0.55264250000000004</v>
       </c>
       <c r="M16">
-        <f>$B$2*K16</f>
-        <v>10</v>
+        <f t="shared" si="4"/>
+        <v>12</v>
       </c>
       <c r="N16">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="O16">
-        <f>MAX(M16 - N16, 0)</f>
-        <v>2</v>
+        <f t="shared" si="5"/>
+        <v>6</v>
       </c>
       <c r="P16">
-        <f>CEILING(O16/E16, 1)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="Q16" s="2">
-        <f>I16*P16</f>
+        <f t="shared" si="7"/>
         <v>5.5264250000000006</v>
       </c>
       <c r="R16">
-        <f>E16*P16 +N16 - M16</f>
-        <v>8</v>
+        <f t="shared" si="8"/>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.4">
@@ -1290,46 +1291,46 @@
         <v>0</v>
       </c>
       <c r="H17" s="1">
-        <f>10.75% * (F17 + G17)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I17" s="2">
-        <f>SUM(F17:H17)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J17" s="2">
-        <f>IF(E17&gt;0, I17/E17, 0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K17">
         <v>1</v>
       </c>
       <c r="L17" s="2">
-        <f>J17*K17</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="M17">
-        <f>$B$2*K17</f>
-        <v>10</v>
+        <f t="shared" si="4"/>
+        <v>12</v>
       </c>
       <c r="N17">
         <v>100</v>
       </c>
       <c r="O17">
-        <f>MAX(M17 - N17, 0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P17">
-        <f>CEILING(O17/E17, 1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Q17" s="2">
-        <f>I17*P17</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="R17">
-        <f>E17*P17 +N17 - M17</f>
-        <v>90</v>
+        <f t="shared" si="8"/>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.4">
@@ -1349,46 +1350,46 @@
         <v>0</v>
       </c>
       <c r="H18" s="1">
-        <f>10.75% * (F18 + G18)</f>
+        <f t="shared" si="0"/>
         <v>1.073925</v>
       </c>
       <c r="I18" s="2">
-        <f>SUM(F18:H18)</f>
+        <f t="shared" si="1"/>
         <v>11.063925000000001</v>
       </c>
       <c r="J18" s="2">
-        <f>IF(E18&gt;0, I18/E18, 0)</f>
+        <f t="shared" si="2"/>
         <v>0.11063925000000001</v>
       </c>
       <c r="K18">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="L18" s="2">
-        <f>J18*K18</f>
-        <v>0.88511400000000007</v>
+        <f t="shared" si="3"/>
+        <v>0.66383550000000002</v>
       </c>
       <c r="M18">
-        <f>$B$2*K18</f>
-        <v>80</v>
+        <f t="shared" si="4"/>
+        <v>72</v>
       </c>
       <c r="N18">
         <v>90</v>
       </c>
       <c r="O18">
-        <f>MAX(M18 - N18, 0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="P18">
-        <f>CEILING(O18/E18, 1)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="Q18" s="2">
-        <f>I18*P18</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="R18">
-        <f>E18*P18 +N18 - M18</f>
-        <v>10</v>
+        <f t="shared" si="8"/>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.4">
@@ -1422,7 +1423,11 @@
       </c>
       <c r="L26" s="2">
         <f>SUM(L5:L24)</f>
-        <v>57.394381249999995</v>
+        <v>57.29470624999999</v>
+      </c>
+      <c r="Q26" s="2">
+        <f>SUM(Q5:Q24)</f>
+        <v>593.608925</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.4">
@@ -1437,6 +1442,13 @@
     <hyperlink ref="D9" r:id="rId2" xr:uid="{0E75646C-94D4-4372-B4C0-3B614C88600E}"/>
     <hyperlink ref="D8" r:id="rId3" xr:uid="{67854B4A-86A2-406E-B1FB-6322A3AED707}"/>
     <hyperlink ref="D18" r:id="rId4" xr:uid="{CBDEE24A-5230-4280-A73C-6CE32D07A16C}"/>
+    <hyperlink ref="D5" r:id="rId5" xr:uid="{33144752-59ED-4721-9641-3912E41D4338}"/>
+    <hyperlink ref="D6" r:id="rId6" xr:uid="{5C132CF4-012A-43BE-BDD0-D584A5C26247}"/>
+    <hyperlink ref="D13" r:id="rId7" xr:uid="{F088C49A-EB77-46F7-B2D0-A1CF1FEC9E9B}"/>
+    <hyperlink ref="D14" r:id="rId8" xr:uid="{1C169F47-3186-4A7C-A17F-C7D639E5F162}"/>
+    <hyperlink ref="D15" r:id="rId9" xr:uid="{43248721-7AED-4B0F-A1ED-016B0377A672}"/>
+    <hyperlink ref="D16" r:id="rId10" xr:uid="{09C8A3F2-8EEA-4BEC-8D6A-F6F45A6803A5}"/>
+    <hyperlink ref="D7" r:id="rId11" xr:uid="{5B86C528-F3F0-49CD-A2E4-31E9D973AD6F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1537,11 +1549,11 @@
         <v>0</v>
       </c>
       <c r="H5" s="1">
-        <f>10.75% * (F5 + G5)</f>
+        <f t="shared" ref="H5:H12" si="0">10.75% * (F5 + G5)</f>
         <v>1.073925</v>
       </c>
       <c r="I5" s="2">
-        <f>SUM(F5:H5)</f>
+        <f t="shared" ref="I5:I12" si="1">SUM(F5:H5)</f>
         <v>11.063925000000001</v>
       </c>
       <c r="J5" s="2">
@@ -1552,30 +1564,30 @@
         <v>1</v>
       </c>
       <c r="L5" s="2">
-        <f>J5*K5</f>
+        <f t="shared" ref="L5:L12" si="2">J5*K5</f>
         <v>5.5319625000000006</v>
       </c>
       <c r="M5">
         <f>'Twitchy Cat'!$B$2*K5</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="N5">
         <v>1</v>
       </c>
       <c r="O5">
-        <f>MAX(M5 - N5, 0)</f>
-        <v>9</v>
+        <f t="shared" ref="O5:O12" si="3">MAX(M5 - N5, 0)</f>
+        <v>11</v>
       </c>
       <c r="P5">
-        <f>CEILING(O5/E5, 1)</f>
-        <v>5</v>
+        <f t="shared" ref="P5:P12" si="4">CEILING(O5/E5, 1)</f>
+        <v>6</v>
       </c>
       <c r="Q5" s="2">
-        <f>I5*P5</f>
-        <v>55.319625000000002</v>
+        <f t="shared" ref="Q5:Q12" si="5">I5*P5</f>
+        <v>66.383550000000014</v>
       </c>
       <c r="R5">
-        <f>E5*P5 +N5 - M5</f>
+        <f t="shared" ref="R5:R12" si="6">E5*P5 +N5 - M5</f>
         <v>1</v>
       </c>
     </row>
@@ -1596,11 +1608,11 @@
         <v>0</v>
       </c>
       <c r="H6" s="1">
-        <f>10.75% * (F6 + G6)</f>
+        <f t="shared" si="0"/>
         <v>0.92342499999999994</v>
       </c>
       <c r="I6" s="2">
-        <f>SUM(F6:H6)</f>
+        <f t="shared" si="1"/>
         <v>9.5134249999999998</v>
       </c>
       <c r="J6" s="2">
@@ -1611,31 +1623,31 @@
         <v>1</v>
       </c>
       <c r="L6" s="2">
-        <f>J6*K6</f>
+        <f t="shared" si="2"/>
         <v>0.31711416666666664</v>
       </c>
       <c r="M6">
         <f>'Twitchy Cat'!$B$2*K6</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="N6">
         <v>28</v>
       </c>
       <c r="O6">
-        <f>MAX(M6 - N6, 0)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="P6">
-        <f>CEILING(O6/E6, 1)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q6" s="2">
-        <f>I6*P6</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="R6">
-        <f>E6*P6 +N6 - M6</f>
-        <v>18</v>
+        <f t="shared" si="6"/>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.4">
@@ -1655,46 +1667,46 @@
         <v>0</v>
       </c>
       <c r="H7" s="1">
-        <f>10.75% * (F7 + G7)</f>
+        <f t="shared" si="0"/>
         <v>1.0535000000000001</v>
       </c>
       <c r="I7" s="2">
-        <f>SUM(F7:H7)</f>
+        <f t="shared" si="1"/>
         <v>10.8535</v>
       </c>
       <c r="J7" s="2">
-        <f>IF(E7&gt;0, I7/E7, 0)</f>
+        <f t="shared" ref="J7:J12" si="7">IF(E7&gt;0, I7/E7, 0)</f>
         <v>1.08535</v>
       </c>
       <c r="K7">
         <v>2</v>
       </c>
       <c r="L7" s="2">
-        <f>J7*K7</f>
+        <f t="shared" si="2"/>
         <v>2.1707000000000001</v>
       </c>
       <c r="M7">
         <f>'Twitchy Cat'!$B$2*K7</f>
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="N7">
         <v>10</v>
       </c>
       <c r="O7">
-        <f>MAX(M7 - N7, 0)</f>
-        <v>10</v>
+        <f t="shared" si="3"/>
+        <v>14</v>
       </c>
       <c r="P7">
-        <f>CEILING(O7/E7, 1)</f>
-        <v>1</v>
+        <f t="shared" si="4"/>
+        <v>2</v>
       </c>
       <c r="Q7" s="2">
-        <f>I7*P7</f>
-        <v>10.8535</v>
+        <f t="shared" si="5"/>
+        <v>21.707000000000001</v>
       </c>
       <c r="R7">
-        <f>E7*P7 +N7 - M7</f>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.4">
@@ -1714,46 +1726,46 @@
         <v>0</v>
       </c>
       <c r="H8" s="1">
-        <f>10.75% * (F8 + G8)</f>
+        <f t="shared" si="0"/>
         <v>1.073925</v>
       </c>
       <c r="I8" s="2">
-        <f>SUM(F8:H8)</f>
+        <f t="shared" si="1"/>
         <v>11.063925000000001</v>
       </c>
       <c r="J8" s="2">
-        <f>IF(E8&gt;0, I8/E8, 0)</f>
+        <f t="shared" si="7"/>
         <v>0.11063925000000001</v>
       </c>
       <c r="K8">
         <v>8</v>
       </c>
       <c r="L8" s="2">
-        <f>J8*K8</f>
+        <f t="shared" si="2"/>
         <v>0.88511400000000007</v>
       </c>
       <c r="M8">
         <f>'Twitchy Cat'!$B$2*K8</f>
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="N8">
         <v>90</v>
       </c>
       <c r="O8">
-        <f>MAX(M8 - N8, 0)</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>6</v>
       </c>
       <c r="P8">
-        <f>CEILING(O8/E8, 1)</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>1</v>
       </c>
       <c r="Q8" s="2">
-        <f>I8*P8</f>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>11.063925000000001</v>
       </c>
       <c r="R8">
-        <f>E8*P8 +N8 - M8</f>
-        <v>10</v>
+        <f t="shared" si="6"/>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.4">
@@ -1773,46 +1785,46 @@
         <v>0</v>
       </c>
       <c r="H9" s="1">
-        <f>10.75% * (F9 + G9)</f>
+        <f t="shared" si="0"/>
         <v>0.85892500000000005</v>
       </c>
       <c r="I9" s="2">
-        <f>SUM(F9:H9)</f>
+        <f t="shared" si="1"/>
         <v>8.8489249999999995</v>
       </c>
       <c r="J9" s="2">
-        <f>IF(E9&gt;0, I9/E9, 0)</f>
+        <f t="shared" si="7"/>
         <v>0.88489249999999997</v>
       </c>
       <c r="K9">
         <v>1</v>
       </c>
       <c r="L9" s="2">
-        <f>J9*K9</f>
+        <f t="shared" si="2"/>
         <v>0.88489249999999997</v>
       </c>
       <c r="M9">
         <f>'Twitchy Cat'!$B$2*K9</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="N9">
         <v>0</v>
       </c>
       <c r="O9">
-        <f>MAX(M9 - N9, 0)</f>
-        <v>10</v>
+        <f t="shared" si="3"/>
+        <v>12</v>
       </c>
       <c r="P9">
-        <f>CEILING(O9/E9, 1)</f>
-        <v>1</v>
+        <f t="shared" si="4"/>
+        <v>2</v>
       </c>
       <c r="Q9" s="2">
-        <f>I9*P9</f>
-        <v>8.8489249999999995</v>
+        <f t="shared" si="5"/>
+        <v>17.697849999999999</v>
       </c>
       <c r="R9">
-        <f>E9*P9 +N9 - M9</f>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.4">
@@ -1832,46 +1844,46 @@
         <v>0</v>
       </c>
       <c r="H10" s="1">
-        <f>10.75% * (F10 + G10)</f>
+        <f t="shared" si="0"/>
         <v>1.009425</v>
       </c>
       <c r="I10" s="2">
-        <f>SUM(F10:H10)</f>
+        <f t="shared" si="1"/>
         <v>10.399425000000001</v>
       </c>
       <c r="J10" s="2">
-        <f>IF(E10&gt;0, I10/E10, 0)</f>
+        <f t="shared" si="7"/>
         <v>1.0399425</v>
       </c>
       <c r="K10">
         <v>1</v>
       </c>
       <c r="L10" s="2">
-        <f>J10*K10</f>
+        <f t="shared" si="2"/>
         <v>1.0399425</v>
       </c>
       <c r="M10">
         <f>'Twitchy Cat'!$B$2*K10</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="N10">
         <v>8</v>
       </c>
       <c r="O10">
-        <f>MAX(M10 - N10, 0)</f>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>4</v>
       </c>
       <c r="P10">
-        <f>CEILING(O10/E10, 1)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="Q10" s="2">
-        <f>I10*P10</f>
+        <f t="shared" si="5"/>
         <v>10.399425000000001</v>
       </c>
       <c r="R10">
-        <f>E10*P10 +N10 - M10</f>
-        <v>8</v>
+        <f t="shared" si="6"/>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.4">
@@ -1891,46 +1903,46 @@
         <v>0</v>
       </c>
       <c r="H11" s="1">
-        <f>10.75% * (F11 + G11)</f>
+        <f t="shared" si="0"/>
         <v>0.53642500000000004</v>
       </c>
       <c r="I11" s="2">
-        <f>SUM(F11:H11)</f>
+        <f t="shared" si="1"/>
         <v>5.5264250000000006</v>
       </c>
       <c r="J11" s="2">
-        <f>IF(E11&gt;0, I11/E11, 0)</f>
+        <f t="shared" si="7"/>
         <v>0.55264250000000004</v>
       </c>
       <c r="K11">
         <v>1</v>
       </c>
       <c r="L11" s="2">
-        <f>J11*K11</f>
+        <f t="shared" si="2"/>
         <v>0.55264250000000004</v>
       </c>
       <c r="M11">
         <f>'Twitchy Cat'!$B$2*K11</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="N11">
         <v>8</v>
       </c>
       <c r="O11">
-        <f>MAX(M11 - N11, 0)</f>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>4</v>
       </c>
       <c r="P11">
-        <f>CEILING(O11/E11, 1)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="Q11" s="2">
-        <f>I11*P11</f>
+        <f t="shared" si="5"/>
         <v>5.5264250000000006</v>
       </c>
       <c r="R11">
-        <f>E11*P11 +N11 - M11</f>
-        <v>8</v>
+        <f t="shared" si="6"/>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.4">
@@ -1950,46 +1962,46 @@
         <v>0</v>
       </c>
       <c r="H12" s="1">
-        <f>10.75% * (F12 + G12)</f>
+        <f t="shared" si="0"/>
         <v>1.073925</v>
       </c>
       <c r="I12" s="2">
-        <f>SUM(F12:H12)</f>
+        <f t="shared" si="1"/>
         <v>11.063925000000001</v>
       </c>
       <c r="J12" s="2">
-        <f>IF(E12&gt;0, I12/E12, 0)</f>
+        <f t="shared" si="7"/>
         <v>1.8439875000000001</v>
       </c>
       <c r="K12">
         <v>1</v>
       </c>
       <c r="L12" s="2">
-        <f>J12*K12</f>
+        <f t="shared" si="2"/>
         <v>1.8439875000000001</v>
       </c>
       <c r="M12">
         <f>'Twitchy Cat'!$B$2*K12</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="N12">
         <v>4</v>
       </c>
       <c r="O12">
-        <f>MAX(M12 - N12, 0)</f>
-        <v>6</v>
+        <f t="shared" si="3"/>
+        <v>8</v>
       </c>
       <c r="P12">
-        <f>CEILING(O12/E12, 1)</f>
-        <v>1</v>
+        <f t="shared" si="4"/>
+        <v>2</v>
       </c>
       <c r="Q12" s="2">
-        <f>I12*P12</f>
-        <v>11.063925000000001</v>
+        <f t="shared" si="5"/>
+        <v>22.127850000000002</v>
       </c>
       <c r="R12">
-        <f>E12*P12 +N12 - M12</f>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.4">
@@ -2002,7 +2014,7 @@
       <c r="O14" s="2"/>
       <c r="Q14" s="2">
         <f>SUM(Q4:Q12)</f>
-        <v>102.01182499999999</v>
+        <v>154.906025</v>
       </c>
     </row>
   </sheetData>

</xml_diff>